<commit_message>
næsten færdig udgave? test
</commit_message>
<xml_diff>
--- a/fravær.xlsx
+++ b/fravær.xlsx
@@ -533,7 +533,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3/18</t>
+          <t>0/18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Til stede</t>
+          <t>Fraværende</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Til stede</t>
+          <t>Fraværende</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Til stede</t>
+          <t>Fraværende</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">

</xml_diff>